<commit_message>
Add initial documentation, fix some properties of map
</commit_message>
<xml_diff>
--- a/assets/d3-geomap/data/incident_counts.xlsx
+++ b/assets/d3-geomap/data/incident_counts.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/d3-geomap/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/privacyincidents/assets/d3-geomap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="2260" windowWidth="28160" windowHeight="16180" tabRatio="500"/>
+    <workbookView xWindow="300" yWindow="1140" windowWidth="28160" windowHeight="16180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>Australia</t>
   </si>
   <si>
-    <t>AUT</t>
-  </si>
-  <si>
     <t>Canada</t>
   </si>
   <si>
@@ -87,6 +84,9 @@
   </si>
   <si>
     <t>WLD</t>
+  </si>
+  <si>
+    <t>AUS</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -425,7 +425,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -433,10 +433,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -444,10 +444,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -455,10 +455,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -466,10 +466,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -477,10 +477,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -488,10 +488,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
       </c>
       <c r="C8">
         <v>9</v>
@@ -499,10 +499,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
       </c>
       <c r="C9">
         <v>53</v>
@@ -510,10 +510,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
       </c>
       <c r="C10">
         <v>79</v>

</xml_diff>